<commit_message>
Adding filter option on input data
</commit_message>
<xml_diff>
--- a/data/Betting.xlsx
+++ b/data/Betting.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25216"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B171A102-0F6B-41C1-BB6C-81799D741DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47C4F3A7-020A-4BC8-BFDB-8C4603C21D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="124">
   <si>
     <t>Købsdato</t>
   </si>
@@ -241,6 +241,153 @@
   </si>
   <si>
     <t>Crystal P - Liverpool</t>
+  </si>
+  <si>
+    <t>Leicester - Liverpool</t>
+  </si>
+  <si>
+    <t>Liverpool - Aston Villa</t>
+  </si>
+  <si>
+    <t>Wolverhampton - Liverpool</t>
+  </si>
+  <si>
+    <t>Hvem vinder 1. halvleg? Liverpool</t>
+  </si>
+  <si>
+    <t>Everton - Liverpool</t>
+  </si>
+  <si>
+    <t>Manchester U - Liverpool</t>
+  </si>
+  <si>
+    <t>4-ling ID 4</t>
+  </si>
+  <si>
+    <t>Wolverhampton - Newcastle</t>
+  </si>
+  <si>
+    <t>4-ling ID 4: X</t>
+  </si>
+  <si>
+    <t>Burnley - Norwich</t>
+  </si>
+  <si>
+    <t>Chelsea - Southampton</t>
+  </si>
+  <si>
+    <t>4-ling ID 4: 1</t>
+  </si>
+  <si>
+    <t>Leeds - Watford</t>
+  </si>
+  <si>
+    <t>Manchester U - Everton</t>
+  </si>
+  <si>
+    <t>Mål mellem 1 - 15 Minutter: Nej</t>
+  </si>
+  <si>
+    <t>Landshold</t>
+  </si>
+  <si>
+    <t>Frankrig - Schweiz</t>
+  </si>
+  <si>
+    <t>Belgien - Portugal</t>
+  </si>
+  <si>
+    <t>Wales - Danmark</t>
+  </si>
+  <si>
+    <t>Rusland - Danmark</t>
+  </si>
+  <si>
+    <t>1. halvleg Hvornår scores det første mål? Ingen mål</t>
+  </si>
+  <si>
+    <t>Mål mellem 16 - 30 Minutter: Nej</t>
+  </si>
+  <si>
+    <t>Vindende hold mellem 1 Og 15 Minutter: Uafgjort</t>
+  </si>
+  <si>
+    <t>England - Skotland</t>
+  </si>
+  <si>
+    <t>Holland - Østrig</t>
+  </si>
+  <si>
+    <t>Danmark - Belgien</t>
+  </si>
+  <si>
+    <t>Italien - Schweiz</t>
+  </si>
+  <si>
+    <t>Begge hold scorer? Nej</t>
+  </si>
+  <si>
+    <t>Frankrig - Tyskland</t>
+  </si>
+  <si>
+    <t>Spanien - Sverige</t>
+  </si>
+  <si>
+    <t>Hjørnespark - O/U 9,5: Over</t>
+  </si>
+  <si>
+    <t>Hjørnespark</t>
+  </si>
+  <si>
+    <t>England - Kroatien</t>
+  </si>
+  <si>
+    <t>Tyrkiet - Italien</t>
+  </si>
+  <si>
+    <t>Hvilket hold scorer 4. mål: Ingen mål</t>
+  </si>
+  <si>
+    <t>Liverpool - Crystal P</t>
+  </si>
+  <si>
+    <t>Hjørnespark - O/U 12,5: Over</t>
+  </si>
+  <si>
+    <t>Antal mål O/U 1,5: Over</t>
+  </si>
+  <si>
+    <t>Burnley - Liverpool</t>
+  </si>
+  <si>
+    <t>West Bromwich - Liverpool</t>
+  </si>
+  <si>
+    <t>Antal mål O/U 2,5: Over</t>
+  </si>
+  <si>
+    <t>Leeds - Liverpool</t>
+  </si>
+  <si>
+    <t>Real Madrid - Liverpool</t>
+  </si>
+  <si>
+    <t>Vindende hold mellem 16 Og 30 Minutter: Uafgjort</t>
+  </si>
+  <si>
+    <t>Manchester U - Brighton</t>
+  </si>
+  <si>
+    <t>Hvilket hold scorer 3. mål: Ingen mål</t>
+  </si>
+  <si>
+    <t>Pengene tilbage ved uafgjort: Manchester U</t>
+  </si>
+  <si>
+    <t>Halvleg/fuldtid Uafgjort / Liverpool</t>
+  </si>
+  <si>
+    <t>Halvleg/fuldtid</t>
   </si>
   <si>
     <t>Total gevinst</t>
@@ -621,11 +768,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1795,6 +1942,1612 @@
         <v>42.707400000000007</v>
       </c>
       <c r="K34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="1">
+        <v>44558</v>
+      </c>
+      <c r="B35" s="1">
+        <v>44558</v>
+      </c>
+      <c r="C35" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35">
+        <v>1.34</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>50</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="1">
+        <v>44541</v>
+      </c>
+      <c r="B36" s="1">
+        <v>44541</v>
+      </c>
+      <c r="C36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36">
+        <v>1.7</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>50</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B37" s="1">
+        <v>44534</v>
+      </c>
+      <c r="C37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37">
+        <v>3.2</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>50</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B38" s="1">
+        <v>44531</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38">
+        <v>1.37</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>100</v>
+      </c>
+      <c r="J38">
+        <f>G38 * I38</f>
+        <v>137</v>
+      </c>
+      <c r="K38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="1">
+        <v>44493</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44493</v>
+      </c>
+      <c r="C39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>50</v>
+      </c>
+      <c r="J39">
+        <f>G39 * I39</f>
+        <v>122.50000000000001</v>
+      </c>
+      <c r="K39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>77</v>
+      </c>
+      <c r="G40">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>10</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>79</v>
+      </c>
+      <c r="G41">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="K41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="K42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B43" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="K43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B44" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s">
+        <v>82</v>
+      </c>
+      <c r="G44">
+        <v>1.18</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="K44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="1">
+        <v>44471</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44471</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45">
+        <v>1.3</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>29</v>
+      </c>
+      <c r="J45">
+        <f>G45 * I45</f>
+        <v>37.700000000000003</v>
+      </c>
+      <c r="K45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B46" s="1">
+        <v>44375</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46">
+        <v>1.58</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>100</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B47" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47">
+        <v>1.82</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>50</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B48" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s">
+        <v>21</v>
+      </c>
+      <c r="G48">
+        <v>3.05</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B49" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49">
+        <v>1.24</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>50</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49:J51" si="0">G49 * I49</f>
+        <v>62</v>
+      </c>
+      <c r="K49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="1">
+        <v>44373</v>
+      </c>
+      <c r="B50" s="1">
+        <v>44373</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" t="s">
+        <v>16</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G50">
+        <v>1.92</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>100</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="K50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B51" s="1">
+        <v>44368</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D51" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G51">
+        <v>1.2</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>200</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="K51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B52" s="1">
+        <v>44368</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D52" t="s">
+        <v>90</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F52" t="s">
+        <v>91</v>
+      </c>
+      <c r="G52">
+        <v>1.42</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>100</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B53" s="1">
+        <v>44368</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s">
+        <v>92</v>
+      </c>
+      <c r="G53">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>100</v>
+      </c>
+      <c r="J53">
+        <f t="shared" ref="J53:J54" si="1">G53 * I53</f>
+        <v>112.99999999999999</v>
+      </c>
+      <c r="K53" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="1">
+        <v>44368</v>
+      </c>
+      <c r="B54" s="1">
+        <v>44368</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54">
+        <v>1.25</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>100</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="K54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B55" s="1">
+        <v>44365</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" t="s">
+        <v>94</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G55">
+        <v>1.65</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>50</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="1">
+        <v>44365</v>
+      </c>
+      <c r="B56" s="1">
+        <v>44365</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" t="s">
+        <v>94</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" t="s">
+        <v>52</v>
+      </c>
+      <c r="G56">
+        <v>1.42</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>50</v>
+      </c>
+      <c r="J56">
+        <f t="shared" ref="J56:J58" si="2">G56 * I56</f>
+        <v>71</v>
+      </c>
+      <c r="K56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B57" s="1">
+        <v>44364</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D57" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G57">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>100</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="2"/>
+        <v>115.99999999999999</v>
+      </c>
+      <c r="K57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B58" s="1">
+        <v>44364</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" t="s">
+        <v>96</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G58">
+        <v>1.18</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>100</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="K58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B59" s="1">
+        <v>44363</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D59" t="s">
+        <v>97</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59">
+        <v>1.4</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>100</v>
+      </c>
+      <c r="J59">
+        <f t="shared" ref="J59:J60" si="3">G59 * I59</f>
+        <v>140</v>
+      </c>
+      <c r="K59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="1">
+        <v>44363</v>
+      </c>
+      <c r="B60" s="1">
+        <v>44363</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G60">
+        <v>1.22</v>
+      </c>
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>100</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="3"/>
+        <v>122</v>
+      </c>
+      <c r="K60" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="1">
+        <v>44362</v>
+      </c>
+      <c r="B61" s="1">
+        <v>44362</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" t="s">
+        <v>99</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>52</v>
+      </c>
+      <c r="G61">
+        <v>1.77</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>100</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B62" s="1">
+        <v>44361</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62">
+        <v>1.27</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>100</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="1">
+        <v>44359</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44359</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s">
+        <v>21</v>
+      </c>
+      <c r="G63">
+        <v>3.9</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+      <c r="J63">
+        <f t="shared" ref="J62:J64" si="4">G63 * I63</f>
+        <v>0</v>
+      </c>
+      <c r="K63" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B64" s="1">
+        <v>44358</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64">
+        <v>1.17</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>50</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="4"/>
+        <v>58.5</v>
+      </c>
+      <c r="K64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="1">
+        <v>44358</v>
+      </c>
+      <c r="B65" s="1">
+        <v>44358</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" t="s">
+        <v>104</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G65">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65">
+        <v>100</v>
+      </c>
+      <c r="J65">
+        <f>G65 * I65</f>
+        <v>109.00000000000001</v>
+      </c>
+      <c r="K65" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B66" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>106</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s">
+        <v>107</v>
+      </c>
+      <c r="G66">
+        <v>1.18</v>
+      </c>
+      <c r="H66">
+        <v>1</v>
+      </c>
+      <c r="I66">
+        <v>50</v>
+      </c>
+      <c r="J66">
+        <f>G66 * I66</f>
+        <v>59</v>
+      </c>
+      <c r="K66" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="1">
+        <v>44339</v>
+      </c>
+      <c r="B67" s="1">
+        <v>44339</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>106</v>
+      </c>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="F67" t="s">
+        <v>108</v>
+      </c>
+      <c r="G67">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H67">
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <v>100</v>
+      </c>
+      <c r="J67">
+        <f>G67 * I67</f>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="K67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="1">
+        <v>44335</v>
+      </c>
+      <c r="B68" s="1">
+        <v>44335</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>25</v>
+      </c>
+      <c r="J68">
+        <f>G68 * I68</f>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="K68" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="1">
+        <v>44332</v>
+      </c>
+      <c r="B69" s="1">
+        <v>44332</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" t="s">
+        <v>110</v>
+      </c>
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G69">
+        <v>1.27</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>25</v>
+      </c>
+      <c r="J69">
+        <f>G69 * I69</f>
+        <v>31.75</v>
+      </c>
+      <c r="K69" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B70" s="1">
+        <v>44329</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>76</v>
+      </c>
+      <c r="E70" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" t="s">
+        <v>111</v>
+      </c>
+      <c r="G70">
+        <v>1.6</v>
+      </c>
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>10</v>
+      </c>
+      <c r="J70">
+        <f>G70 * I70</f>
+        <v>16</v>
+      </c>
+      <c r="K70" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B71" s="1">
+        <v>44329</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" t="s">
+        <v>21</v>
+      </c>
+      <c r="G71">
+        <v>3.65</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>10</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B72" s="1">
+        <v>44305</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D72" t="s">
+        <v>112</v>
+      </c>
+      <c r="E72" t="s">
+        <v>13</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G72">
+        <v>1.52</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>100</v>
+      </c>
+      <c r="J72">
+        <f>G72 * I72</f>
+        <v>152</v>
+      </c>
+      <c r="K72" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B73" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D73" t="s">
+        <v>113</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+      <c r="F73" t="s">
+        <v>114</v>
+      </c>
+      <c r="G73">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73">
+        <v>100</v>
+      </c>
+      <c r="J73">
+        <v>0</v>
+      </c>
+      <c r="K73" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B74" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D74" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" t="s">
+        <v>16</v>
+      </c>
+      <c r="F74" t="s">
+        <v>52</v>
+      </c>
+      <c r="G74">
+        <v>2.15</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>50</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B75" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" t="s">
+        <v>16</v>
+      </c>
+      <c r="F75" t="s">
+        <v>85</v>
+      </c>
+      <c r="G75">
+        <v>1.33</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+      <c r="I75">
+        <v>45</v>
+      </c>
+      <c r="J75">
+        <f>G75 * I75</f>
+        <v>59.85</v>
+      </c>
+      <c r="K75" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B76" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" t="s">
+        <v>115</v>
+      </c>
+      <c r="E76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" t="s">
+        <v>116</v>
+      </c>
+      <c r="G76">
+        <v>1.6</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>100</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B77" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" t="s">
+        <v>115</v>
+      </c>
+      <c r="E77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
+        <v>117</v>
+      </c>
+      <c r="G77">
+        <v>1.28</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="I77">
+        <v>100</v>
+      </c>
+      <c r="J77">
+        <f>G77 * I77</f>
+        <v>128</v>
+      </c>
+      <c r="K77" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B78" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" t="s">
+        <v>115</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G78">
+        <v>1.97</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>50</v>
+      </c>
+      <c r="J78">
+        <v>14.62</v>
+      </c>
+      <c r="K78" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B79" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" t="s">
+        <v>13</v>
+      </c>
+      <c r="F79" t="s">
+        <v>118</v>
+      </c>
+      <c r="G79">
+        <v>4.8</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79">
+        <v>50</v>
+      </c>
+      <c r="J79">
+        <f>G79 * I79</f>
+        <v>240</v>
+      </c>
+      <c r="K79" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B80" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" t="s">
+        <v>51</v>
+      </c>
+      <c r="E80" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" t="s">
+        <v>52</v>
+      </c>
+      <c r="G80">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="I80">
+        <v>50</v>
+      </c>
+      <c r="J80">
+        <f>G80 * I80</f>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="K80" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1820,34 +3573,34 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4">
         <f xml:space="preserve"> SUM(Odds!J:J)</f>
-        <v>1426.2273999999998</v>
+        <v>4171.1473999999998</v>
       </c>
       <c r="B2">
         <f xml:space="preserve"> SUM(Odds!I:I)</f>
-        <v>1333.53</v>
+        <v>4187.53</v>
       </c>
       <c r="C2">
         <f>A2 - B2</f>
-        <v>92.697399999999789</v>
+        <v>-16.382599999999911</v>
       </c>
       <c r="D2">
         <f>ROUND(100 * (C2 / B2), 2)</f>
-        <v>6.95</v>
+        <v>-0.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>